<commit_message>
add res boundary attack for SEED 1337
</commit_message>
<xml_diff>
--- a/results/SEED_1337/result.xlsx
+++ b/results/SEED_1337/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -800,115 +852,115 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.523552417755127</v>
+        <v>5.523550033569336</v>
       </c>
       <c r="D4" t="n">
-        <v>4.989015579223633</v>
+        <v>4.989018440246582</v>
       </c>
       <c r="E4" t="n">
-        <v>5.023521163246849</v>
+        <v>5.023545828732577</v>
       </c>
       <c r="F4" t="n">
-        <v>4.651863791725853</v>
+        <v>4.651914423162287</v>
       </c>
       <c r="G4" t="n">
-        <v>4.435453371568159</v>
+        <v>4.435529362071644</v>
       </c>
       <c r="H4" t="n">
-        <v>4.448381467299028</v>
+        <v>4.448482556776567</v>
       </c>
       <c r="I4" t="n">
-        <v>4.69308200749484</v>
+        <v>4.693207740783691</v>
       </c>
       <c r="J4" t="n">
-        <v>6.064794952219183</v>
+        <v>6.064614556052468</v>
       </c>
       <c r="K4" t="n">
-        <v>8.154313629323786</v>
+        <v>8.154090057719838</v>
       </c>
       <c r="L4" t="n">
-        <v>17.12062267823653</v>
+        <v>17.12031115185131</v>
       </c>
       <c r="M4" t="n">
-        <v>5.621900948611173</v>
+        <v>5.621898564425382</v>
       </c>
       <c r="N4" t="n">
-        <v>5.806862094185569</v>
+        <v>5.806861357255415</v>
       </c>
       <c r="O4" t="n">
-        <v>6.092842275446111</v>
+        <v>6.092840541492809</v>
       </c>
       <c r="P4" t="n">
-        <v>6.450304811651057</v>
+        <v>6.450303467837247</v>
       </c>
       <c r="Q4" t="n">
-        <v>6.884694706309926</v>
+        <v>6.884694511240179</v>
       </c>
       <c r="R4" t="n">
-        <v>8.244660160758279</v>
+        <v>8.244659185409546</v>
       </c>
       <c r="S4" t="n">
-        <v>9.885632384907115</v>
+        <v>9.885632059790872</v>
       </c>
       <c r="T4" t="n">
-        <v>17.54667284271934</v>
+        <v>17.54667388309132</v>
       </c>
       <c r="U4" t="n">
-        <v>5.621900948611173</v>
+        <v>5.621898564425382</v>
       </c>
       <c r="V4" t="n">
-        <v>5.825175328688188</v>
+        <v>5.825174201618541</v>
       </c>
       <c r="W4" t="n">
-        <v>6.142595074393532</v>
+        <v>6.142593643882058</v>
       </c>
       <c r="X4" t="n">
-        <v>6.536285010251132</v>
+        <v>6.536283536390825</v>
       </c>
       <c r="Y4" t="n">
-        <v>7.013604922728105</v>
+        <v>7.013603947379372</v>
       </c>
       <c r="Z4" t="n">
-        <v>8.173859596252441</v>
+        <v>8.173858339136297</v>
       </c>
       <c r="AA4" t="n">
-        <v>10.25403432412581</v>
+        <v>10.25403347882357</v>
       </c>
       <c r="AB4" t="n">
-        <v>18.09528045220809</v>
+        <v>18.09528101574291</v>
       </c>
       <c r="AC4" t="n">
-        <v>6.627487659454346</v>
+        <v>6.627485752105713</v>
       </c>
       <c r="AD4" t="n">
-        <v>7.767051219940186</v>
+        <v>7.767050266265869</v>
       </c>
       <c r="AE4" t="n">
-        <v>8.90921688079834</v>
+        <v>8.909215927124023</v>
       </c>
       <c r="AF4" t="n">
         <v>10.05378818511963</v>
       </c>
       <c r="AG4" t="n">
-        <v>11.20066547393799</v>
+        <v>11.20066452026367</v>
       </c>
       <c r="AH4" t="n">
         <v>14.07552242279053</v>
       </c>
       <c r="AI4" t="n">
-        <v>16.959716796875</v>
+        <v>16.95971870422363</v>
       </c>
       <c r="AJ4" t="n">
         <v>28.5583667755127</v>
       </c>
       <c r="AK4" t="n">
-        <v>6.741440296173096</v>
+        <v>6.741439819335938</v>
       </c>
       <c r="AL4" t="n">
-        <v>7.963371753692627</v>
+        <v>7.963369369506836</v>
       </c>
       <c r="AM4" t="n">
-        <v>9.189281463623047</v>
+        <v>9.189279556274414</v>
       </c>
       <c r="AN4" t="n">
         <v>10.41890621185303</v>
@@ -923,7 +975,31 @@
         <v>17.85449409484863</v>
       </c>
       <c r="AR4" t="n">
-        <v>30.35847282409668</v>
+        <v>30.35847663879395</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>5.556640148162842</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>5.59864616394043</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>5.652719497680664</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>5.719746112823486</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>5.748430728912354</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>5.866903305053711</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>6.338736057281494</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7.508411884307861</v>
       </c>
     </row>
     <row r="5">
@@ -934,118 +1010,118 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6.826283361482293</v>
+        <v>6.826280846769682</v>
       </c>
       <c r="D5" t="n">
-        <v>6.335457027481941</v>
+        <v>6.335460640193221</v>
       </c>
       <c r="E5" t="n">
-        <v>6.295028597662801</v>
+        <v>6.295047183393922</v>
       </c>
       <c r="F5" t="n">
-        <v>5.940504430680784</v>
+        <v>5.940537674512687</v>
       </c>
       <c r="G5" t="n">
-        <v>5.791177066010976</v>
+        <v>5.791213352205387</v>
       </c>
       <c r="H5" t="n">
-        <v>5.863306360032136</v>
+        <v>5.863336345566226</v>
       </c>
       <c r="I5" t="n">
-        <v>6.146437933116026</v>
+        <v>6.146451508860616</v>
       </c>
       <c r="J5" t="n">
-        <v>7.555664403507134</v>
+        <v>7.55561864916307</v>
       </c>
       <c r="K5" t="n">
-        <v>9.565427854848776</v>
+        <v>9.565322789194516</v>
       </c>
       <c r="L5" t="n">
-        <v>18.74468342323624</v>
+        <v>18.74444738716356</v>
       </c>
       <c r="M5" t="n">
-        <v>6.903600186820501</v>
+        <v>6.903598089052354</v>
       </c>
       <c r="N5" t="n">
-        <v>7.093141120347238</v>
+        <v>7.093139802748771</v>
       </c>
       <c r="O5" t="n">
-        <v>7.386317773312517</v>
+        <v>7.386316618660216</v>
       </c>
       <c r="P5" t="n">
-        <v>7.774207963504029</v>
+        <v>7.774206242000623</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.244309634953998</v>
+        <v>8.244308822120489</v>
       </c>
       <c r="R5" t="n">
-        <v>9.696794574872799</v>
+        <v>9.696793431847064</v>
       </c>
       <c r="S5" t="n">
-        <v>11.44219141873922</v>
+        <v>11.44219073800565</v>
       </c>
       <c r="T5" t="n">
-        <v>19.58255191094523</v>
+        <v>19.58255250993878</v>
       </c>
       <c r="U5" t="n">
-        <v>6.903600186820501</v>
+        <v>6.903598089052354</v>
       </c>
       <c r="V5" t="n">
-        <v>7.112837950958211</v>
+        <v>7.112836344953103</v>
       </c>
       <c r="W5" t="n">
-        <v>7.437959892744439</v>
+        <v>7.437958515570088</v>
       </c>
       <c r="X5" t="n">
-        <v>7.871388482229773</v>
+        <v>7.87138695407789</v>
       </c>
       <c r="Y5" t="n">
-        <v>8.397130818183891</v>
+        <v>8.397129855968094</v>
       </c>
       <c r="Z5" t="n">
-        <v>9.663573814910169</v>
+        <v>9.663572846290247</v>
       </c>
       <c r="AA5" t="n">
-        <v>11.94179038548564</v>
+        <v>11.94178929416395</v>
       </c>
       <c r="AB5" t="n">
-        <v>20.7486921773032</v>
+        <v>20.7486929209789</v>
       </c>
       <c r="AC5" t="n">
-        <v>7.747431421705726</v>
+        <v>7.747429698367863</v>
       </c>
       <c r="AD5" t="n">
-        <v>8.723582470136982</v>
+        <v>8.723581158279989</v>
       </c>
       <c r="AE5" t="n">
-        <v>9.739030976705761</v>
+        <v>9.739028626555484</v>
       </c>
       <c r="AF5" t="n">
-        <v>10.78336284776881</v>
+        <v>10.78336143273805</v>
       </c>
       <c r="AG5" t="n">
-        <v>11.84960213166294</v>
+        <v>11.84960084395811</v>
       </c>
       <c r="AH5" t="n">
         <v>14.58028887259777</v>
       </c>
       <c r="AI5" t="n">
-        <v>17.37116094755948</v>
+        <v>17.37116270435494</v>
       </c>
       <c r="AJ5" t="n">
-        <v>28.80628089232722</v>
+        <v>28.8062840705483</v>
       </c>
       <c r="AK5" t="n">
-        <v>7.82414976138145</v>
+        <v>7.82414829871864</v>
       </c>
       <c r="AL5" t="n">
-        <v>8.882358562912033</v>
+        <v>8.882356845036041</v>
       </c>
       <c r="AM5" t="n">
-        <v>9.983153840130038</v>
+        <v>9.983152693789648</v>
       </c>
       <c r="AN5" t="n">
-        <v>11.11494454270915</v>
+        <v>11.11494248348289</v>
       </c>
       <c r="AO5" t="n">
         <v>12.2700771925658</v>
@@ -1054,10 +1130,34 @@
         <v>15.22711014680237</v>
       </c>
       <c r="AQ5" t="n">
-        <v>18.24658087486658</v>
+        <v>18.24658003861186</v>
       </c>
       <c r="AR5" t="n">
-        <v>30.61481614796074</v>
+        <v>30.61481714478455</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>6.851199759229703</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>6.873898227145802</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>6.906926048641773</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>7.001195260589745</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>7.036477819980958</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>7.238478351674214</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>7.796053734223764</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>9.321373724815231</v>
       </c>
     </row>
     <row r="6">
@@ -1068,85 +1168,85 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9995709657669067</v>
+        <v>0.9995708465576172</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9996910691261292</v>
+        <v>0.9996911883354187</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9995656609535217</v>
+        <v>0.9995654225349426</v>
       </c>
       <c r="F6" t="n">
         <v>0.9995379447937012</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9994891285896301</v>
+        <v>0.9994890689849854</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9994188547134399</v>
+        <v>0.9994187355041504</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9993272423744202</v>
+        <v>0.9993270039558411</v>
       </c>
       <c r="J6" t="n">
-        <v>0.99900883436203</v>
+        <v>0.9990085959434509</v>
       </c>
       <c r="K6" t="n">
         <v>0.9985573291778564</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9955934882164001</v>
+        <v>0.9955933690071106</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9995701909065247</v>
+        <v>0.9995699524879456</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9995399713516235</v>
+        <v>0.999539852142334</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9994803667068481</v>
+        <v>0.9994803071022034</v>
       </c>
       <c r="P6" t="n">
         <v>0.9993910193443298</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9992714524269104</v>
+        <v>0.9992713928222656</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9988403916358948</v>
+        <v>0.9988402724266052</v>
       </c>
       <c r="S6" t="n">
-        <v>0.998215913772583</v>
+        <v>0.9982157945632935</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9938497543334961</v>
+        <v>0.9938496351242065</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9995701909065247</v>
+        <v>0.9995699524879456</v>
       </c>
       <c r="V6" t="n">
-        <v>0.9995394349098206</v>
+        <v>0.9995392560958862</v>
       </c>
       <c r="W6" t="n">
         <v>0.9994805455207825</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9993919134140015</v>
+        <v>0.9993916749954224</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.9992732405662537</v>
+        <v>0.9992731213569641</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.9989446997642517</v>
+        <v>0.9989445805549622</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.9982227683067322</v>
+        <v>0.9982226490974426</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.9939936399459839</v>
+        <v>0.9939937591552734</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.9994674921035767</v>
+        <v>0.9994674324989319</v>
       </c>
       <c r="AD6" t="n">
         <v>0.9993349313735962</v>
@@ -1155,43 +1255,67 @@
         <v>0.9991727471351624</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.9989801049232483</v>
+        <v>0.9989799857139587</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.9987556338310242</v>
+        <v>0.9987555146217346</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.9980526566505432</v>
+        <v>0.9980525374412537</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.9971358776092529</v>
+        <v>0.9971356391906738</v>
       </c>
       <c r="AJ6" t="n">
         <v>0.9910988211631775</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.9994464516639709</v>
+        <v>0.9994461536407471</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.9992853403091431</v>
+        <v>0.9992852807044983</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.9990874528884888</v>
+        <v>0.9990873336791992</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.99885094165802</v>
+        <v>0.9988508820533752</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.9985753893852234</v>
+        <v>0.9985752701759338</v>
       </c>
       <c r="AP6" t="n">
         <v>0.9977079629898071</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.9965738654136658</v>
+        <v>0.9965736269950867</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.98908931016922</v>
+        <v>0.9890891909599304</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.9995687007904053</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.999567985534668</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9995618462562561</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9995406270027161</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995287656784058</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9994986653327942</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9993953108787537</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9991246461868286</v>
       </c>
     </row>
     <row r="7">
@@ -1206,130 +1330,154 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.056714773178101</v>
+        <v>3.056711435317993</v>
       </c>
       <c r="D7" t="n">
-        <v>2.312292098999023</v>
+        <v>2.312292575836182</v>
       </c>
       <c r="E7" t="n">
-        <v>3.094857909462668</v>
+        <v>3.094854831695557</v>
       </c>
       <c r="F7" t="n">
-        <v>3.143668391487815</v>
+        <v>3.14366626739502</v>
       </c>
       <c r="G7" t="n">
-        <v>3.198293815959584</v>
+        <v>3.198290738192472</v>
       </c>
       <c r="H7" t="n">
-        <v>3.262979247353293</v>
+        <v>3.262976776469837</v>
       </c>
       <c r="I7" t="n">
-        <v>3.333612832156095</v>
+        <v>3.333608887412332</v>
       </c>
       <c r="J7" t="n">
-        <v>3.549160740592263</v>
+        <v>3.549158919941295</v>
       </c>
       <c r="K7" t="n">
-        <v>3.878682526675138</v>
+        <v>3.878679709001021</v>
       </c>
       <c r="L7" t="n">
-        <v>5.903695019808683</v>
+        <v>5.903694109483198</v>
       </c>
       <c r="M7" t="n">
-        <v>3.197227738120339</v>
+        <v>3.197224270213734</v>
       </c>
       <c r="N7" t="n">
-        <v>3.584021351554177</v>
+        <v>3.584017406810414</v>
       </c>
       <c r="O7" t="n">
-        <v>4.185018799521706</v>
+        <v>4.185016437010332</v>
       </c>
       <c r="P7" t="n">
-        <v>4.901570493524725</v>
+        <v>4.901568109338934</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.706804665652188</v>
+        <v>5.706804990768433</v>
       </c>
       <c r="R7" t="n">
-        <v>7.901909004558217</v>
+        <v>7.9019089828838</v>
       </c>
       <c r="S7" t="n">
-        <v>10.2741058956493</v>
+        <v>10.27410466020758</v>
       </c>
       <c r="T7" t="n">
-        <v>19.86626003005288</v>
+        <v>19.86625987833196</v>
       </c>
       <c r="U7" t="n">
-        <v>3.094857909462668</v>
+        <v>3.094854831695557</v>
       </c>
       <c r="V7" t="n">
-        <v>3.144738847559148</v>
+        <v>3.144734902815385</v>
       </c>
       <c r="W7" t="n">
-        <v>3.199398084120317</v>
+        <v>3.199395353143865</v>
       </c>
       <c r="X7" t="n">
-        <v>3.264049486680464</v>
+        <v>3.264047492634166</v>
       </c>
       <c r="Y7" t="n">
-        <v>3.333464882590554</v>
+        <v>3.333462238311768</v>
       </c>
       <c r="Z7" t="n">
-        <v>3.504064689983021</v>
+        <v>3.50406044179743</v>
       </c>
       <c r="AA7" t="n">
-        <v>3.901561173525724</v>
+        <v>3.901557879014449</v>
       </c>
       <c r="AB7" t="n">
-        <v>6.05706921490756</v>
+        <v>6.057067350907759</v>
       </c>
       <c r="AC7" t="n">
-        <v>4.37489128112793</v>
+        <v>4.374887466430664</v>
       </c>
       <c r="AD7" t="n">
-        <v>5.732235431671143</v>
+        <v>5.732231140136719</v>
       </c>
       <c r="AE7" t="n">
-        <v>7.091312885284424</v>
+        <v>7.091310024261475</v>
       </c>
       <c r="AF7" t="n">
-        <v>8.452170372009277</v>
+        <v>8.452167510986328</v>
       </c>
       <c r="AG7" t="n">
-        <v>9.8133544921875</v>
+        <v>9.813350677490234</v>
       </c>
       <c r="AH7" t="n">
-        <v>13.21981811523438</v>
+        <v>13.21981525421143</v>
       </c>
       <c r="AI7" t="n">
-        <v>16.62668609619141</v>
+        <v>16.62668418884277</v>
       </c>
       <c r="AJ7" t="n">
         <v>30.2068977355957</v>
       </c>
       <c r="AK7" t="n">
-        <v>4.590685844421387</v>
+        <v>4.590683460235596</v>
       </c>
       <c r="AL7" t="n">
-        <v>6.126983165740967</v>
+        <v>6.126980304718018</v>
       </c>
       <c r="AM7" t="n">
-        <v>7.665304183959961</v>
+        <v>7.665301322937012</v>
       </c>
       <c r="AN7" t="n">
-        <v>9.204474449157715</v>
+        <v>9.204471588134766</v>
       </c>
       <c r="AO7" t="n">
-        <v>10.74240398406982</v>
+        <v>10.74240207672119</v>
       </c>
       <c r="AP7" t="n">
-        <v>14.58688068389893</v>
+        <v>14.58687973022461</v>
       </c>
       <c r="AQ7" t="n">
-        <v>18.4229679107666</v>
+        <v>18.42296600341797</v>
       </c>
       <c r="AR7" t="n">
-        <v>33.55676651000977</v>
+        <v>33.55677032470703</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3.110022068023682</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>3.213740348815918</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.311930179595947</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>3.568376064300537</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>3.810426950454712</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>4.92809534072876</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>5.25084400177002</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>8.721148490905762</v>
       </c>
     </row>
     <row r="8">
@@ -1340,130 +1488,154 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.023079569182133</v>
+        <v>4.023075539316152</v>
       </c>
       <c r="D8" t="n">
-        <v>3.261153084136252</v>
+        <v>3.261153376570936</v>
       </c>
       <c r="E8" t="n">
-        <v>4.059533004038046</v>
+        <v>4.059529504939906</v>
       </c>
       <c r="F8" t="n">
-        <v>4.106869545648022</v>
+        <v>4.106866624929791</v>
       </c>
       <c r="G8" t="n">
-        <v>4.165522112454549</v>
+        <v>4.165519742849083</v>
       </c>
       <c r="H8" t="n">
-        <v>4.238944952562131</v>
+        <v>4.238941814574028</v>
       </c>
       <c r="I8" t="n">
-        <v>4.324787518427918</v>
+        <v>4.324783115612606</v>
       </c>
       <c r="J8" t="n">
-        <v>4.603972102238274</v>
+        <v>4.603968854893234</v>
       </c>
       <c r="K8" t="n">
-        <v>4.999020564639172</v>
+        <v>4.99901691418872</v>
       </c>
       <c r="L8" t="n">
-        <v>7.477681133072131</v>
+        <v>7.477679172352842</v>
       </c>
       <c r="M8" t="n">
-        <v>4.139129710335152</v>
+        <v>4.139126605136521</v>
       </c>
       <c r="N8" t="n">
-        <v>4.508019325106095</v>
+        <v>4.508014734265998</v>
       </c>
       <c r="O8" t="n">
-        <v>5.075553935735618</v>
+        <v>5.075551380896103</v>
       </c>
       <c r="P8" t="n">
-        <v>5.78526546655131</v>
+        <v>5.785262470986788</v>
       </c>
       <c r="Q8" t="n">
-        <v>6.591626860180815</v>
+        <v>6.591626669879183</v>
       </c>
       <c r="R8" t="n">
-        <v>8.851428852543135</v>
+        <v>8.851427887189352</v>
       </c>
       <c r="S8" t="n">
-        <v>11.29561208051082</v>
+        <v>11.29561083877754</v>
       </c>
       <c r="T8" t="n">
-        <v>21.50938135133481</v>
+        <v>21.50938095788165</v>
       </c>
       <c r="U8" t="n">
-        <v>4.059533004038046</v>
+        <v>4.059529504939906</v>
       </c>
       <c r="V8" t="n">
-        <v>4.107621095079575</v>
+        <v>4.107616365650673</v>
       </c>
       <c r="W8" t="n">
-        <v>4.165847002943964</v>
+        <v>4.165843954384778</v>
       </c>
       <c r="X8" t="n">
-        <v>4.238870540711681</v>
+        <v>4.238867575497354</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.323383058696059</v>
+        <v>4.32337930740925</v>
       </c>
       <c r="Z8" t="n">
-        <v>4.543133840324669</v>
+        <v>4.543129444188389</v>
       </c>
       <c r="AA8" t="n">
-        <v>5.015983657237584</v>
+        <v>5.015979427899834</v>
       </c>
       <c r="AB8" t="n">
-        <v>7.56206186789406</v>
+        <v>7.56205830521909</v>
       </c>
       <c r="AC8" t="n">
-        <v>5.105510218246855</v>
+        <v>5.105506855969117</v>
       </c>
       <c r="AD8" t="n">
-        <v>6.297902366562219</v>
+        <v>6.297898126596546</v>
       </c>
       <c r="AE8" t="n">
-        <v>7.549175283091127</v>
+        <v>7.549172503868491</v>
       </c>
       <c r="AF8" t="n">
-        <v>8.835250166679634</v>
+        <v>8.83524757612628</v>
       </c>
       <c r="AG8" t="n">
-        <v>10.14234662833974</v>
+        <v>10.1423428671806</v>
       </c>
       <c r="AH8" t="n">
-        <v>13.46475082467209</v>
+        <v>13.46474855819267</v>
       </c>
       <c r="AI8" t="n">
-        <v>16.82682286628814</v>
+        <v>16.82682105266117</v>
       </c>
       <c r="AJ8" t="n">
-        <v>30.37006152787695</v>
+        <v>30.37006353759148</v>
       </c>
       <c r="AK8" t="n">
-        <v>5.268398199859722</v>
+        <v>5.268395665608677</v>
       </c>
       <c r="AL8" t="n">
-        <v>6.639900293635728</v>
+        <v>6.639897133823227</v>
       </c>
       <c r="AM8" t="n">
-        <v>8.074641585293866</v>
+        <v>8.074637805858588</v>
       </c>
       <c r="AN8" t="n">
-        <v>9.544233040867082</v>
+        <v>9.544230642750192</v>
       </c>
       <c r="AO8" t="n">
-        <v>11.03362682985553</v>
+        <v>11.03362371825127</v>
       </c>
       <c r="AP8" t="n">
-        <v>14.80708001363785</v>
+        <v>14.80707795262513</v>
       </c>
       <c r="AQ8" t="n">
-        <v>18.61017935525517</v>
+        <v>18.61017853533887</v>
       </c>
       <c r="AR8" t="n">
         <v>33.78181551619618</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>4.071732579021903</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>4.128585644186968</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>4.2811606738942</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>4.525118553336799</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>4.96409821033691</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>6.171929081547072</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>6.723516999842268</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>10.96698070721926</v>
       </c>
     </row>
     <row r="9">
@@ -1477,115 +1649,115 @@
         <v>0.9997681975364685</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9998719692230225</v>
+        <v>0.9998718500137329</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9997663497924805</v>
+        <v>0.99976646900177</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9997631907463074</v>
+        <v>0.9997629523277283</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9997581243515015</v>
+        <v>0.9997580051422119</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9997513294219971</v>
+        <v>0.9997512102127075</v>
       </c>
       <c r="I9" t="n">
         <v>0.9997428059577942</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9997127652168274</v>
+        <v>0.9997127056121826</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9996654987335205</v>
+        <v>0.9996654391288757</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9992898106575012</v>
+        <v>0.9992896318435669</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9997560977935791</v>
+        <v>0.9997559785842896</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9997031092643738</v>
+        <v>0.9997029900550842</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9996093511581421</v>
+        <v>0.999609112739563</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9994741678237915</v>
+        <v>0.999474048614502</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9992977380752563</v>
+        <v>0.9992976188659668</v>
       </c>
       <c r="R9" t="n">
-        <v>0.9986760020256042</v>
+        <v>0.9986758828163147</v>
       </c>
       <c r="S9" t="n">
         <v>0.997795581817627</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9917738437652588</v>
+        <v>0.9917737245559692</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9997663497924805</v>
+        <v>0.99976646900177</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9997629523277283</v>
+        <v>0.9997630715370178</v>
       </c>
       <c r="W9" t="n">
         <v>0.9997586607933044</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9997526407241821</v>
+        <v>0.9997525215148926</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.9997456669807434</v>
+        <v>0.9997455477714539</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.999725878238678</v>
+        <v>0.9997257590293884</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.9996789693832397</v>
+        <v>0.999678909778595</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.9993758201599121</v>
+        <v>0.9993757009506226</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.9996401071548462</v>
+        <v>0.9996400475502014</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9994585514068604</v>
+        <v>0.9994584321975708</v>
       </c>
       <c r="AE9" t="n">
         <v>0.9992222189903259</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.9989302754402161</v>
+        <v>0.998930037021637</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9985817670822144</v>
+        <v>0.9985816478729248</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.997454822063446</v>
+        <v>0.9974547028541565</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.9959501624107361</v>
+        <v>0.9959500432014465</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.9858841896057129</v>
+        <v>0.9858840107917786</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.9996060729026794</v>
+        <v>0.9996059536933899</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.9993690848350525</v>
+        <v>0.9993690252304077</v>
       </c>
       <c r="AM9" t="n">
         <v>0.9990560412406921</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.9986655712127686</v>
+        <v>0.998665452003479</v>
       </c>
       <c r="AO9" t="n">
         <v>0.9981974959373474</v>
@@ -1594,10 +1766,34 @@
         <v>0.9966759085655212</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.9946390986442566</v>
+        <v>0.994638979434967</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.9811753630638123</v>
+        <v>0.981175422668457</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0.9997629523277283</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.999753475189209</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.999733567237854</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996894598007202</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9996153712272644</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9993732571601868</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9992401599884033</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9979406595230103</v>
       </c>
     </row>
     <row r="10">
@@ -1612,82 +1808,82 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.474456071853638</v>
+        <v>3.4744553565979</v>
       </c>
       <c r="D10" t="n">
-        <v>1.812993884086609</v>
+        <v>1.81299352645874</v>
       </c>
       <c r="E10" t="n">
-        <v>3.627029288898815</v>
+        <v>3.627030069177801</v>
       </c>
       <c r="F10" t="n">
-        <v>3.995282476598566</v>
+        <v>3.995282780040394</v>
       </c>
       <c r="G10" t="n">
-        <v>4.544564507224343</v>
+        <v>4.544565244154497</v>
       </c>
       <c r="H10" t="n">
-        <v>5.238711552186445</v>
+        <v>5.238712505860762</v>
       </c>
       <c r="I10" t="n">
-        <v>6.032925670797175</v>
+        <v>6.032926256006414</v>
       </c>
       <c r="J10" t="n">
-        <v>8.28658973086964</v>
+        <v>8.286590467799794</v>
       </c>
       <c r="K10" t="n">
-        <v>10.75759367509322</v>
+        <v>10.75759426030246</v>
       </c>
       <c r="L10" t="n">
-        <v>20.67092344977639</v>
+        <v>20.67092433842746</v>
       </c>
       <c r="M10" t="n">
-        <v>3.519490415399725</v>
+        <v>3.519490458748557</v>
       </c>
       <c r="N10" t="n">
-        <v>3.57396988435225</v>
+        <v>3.573970664631237</v>
       </c>
       <c r="O10" t="n">
-        <v>3.64259164983576</v>
+        <v>3.642592300068249</v>
       </c>
       <c r="P10" t="n">
-        <v>3.729272495616566</v>
+        <v>3.729272885756059</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.830647295171564</v>
+        <v>3.830646731636741</v>
       </c>
       <c r="R10" t="n">
-        <v>4.183937506242231</v>
+        <v>4.183939153497869</v>
       </c>
       <c r="S10" t="n">
-        <v>4.693151040510698</v>
+        <v>4.693151647394354</v>
       </c>
       <c r="T10" t="n">
-        <v>7.58193319494074</v>
+        <v>7.581933563405817</v>
       </c>
       <c r="U10" t="n">
-        <v>3.627029288898815</v>
+        <v>3.627030069177801</v>
       </c>
       <c r="V10" t="n">
-        <v>4.003077333623713</v>
+        <v>4.003077767112038</v>
       </c>
       <c r="W10" t="n">
-        <v>4.551761323755438</v>
+        <v>4.551761107011274</v>
       </c>
       <c r="X10" t="n">
-        <v>5.239139860326594</v>
+        <v>5.239141052419489</v>
       </c>
       <c r="Y10" t="n">
-        <v>6.016172279011119</v>
+        <v>6.016172669150612</v>
       </c>
       <c r="Z10" t="n">
-        <v>7.774696718562733</v>
+        <v>7.774696956981312</v>
       </c>
       <c r="AA10" t="n">
-        <v>10.71815646778454</v>
+        <v>10.71815661950545</v>
       </c>
       <c r="AB10" t="n">
-        <v>20.56736831231551</v>
+        <v>20.56736833398992</v>
       </c>
       <c r="AC10" t="n">
         <v>4.533195972442627</v>
@@ -1696,16 +1892,16 @@
         <v>5.842660427093506</v>
       </c>
       <c r="AE10" t="n">
-        <v>7.211223125457764</v>
+        <v>7.211222648620605</v>
       </c>
       <c r="AF10" t="n">
-        <v>8.57909107208252</v>
+        <v>8.579092025756836</v>
       </c>
       <c r="AG10" t="n">
-        <v>9.944443702697754</v>
+        <v>9.944445610046387</v>
       </c>
       <c r="AH10" t="n">
-        <v>13.34742736816406</v>
+        <v>13.34742641448975</v>
       </c>
       <c r="AI10" t="n">
         <v>16.72924423217773</v>
@@ -1714,7 +1910,7 @@
         <v>29.82804107666016</v>
       </c>
       <c r="AK10" t="n">
-        <v>4.879788398742676</v>
+        <v>4.879787921905518</v>
       </c>
       <c r="AL10" t="n">
         <v>6.287019729614258</v>
@@ -1723,7 +1919,7 @@
         <v>7.695785522460938</v>
       </c>
       <c r="AN10" t="n">
-        <v>9.104992866516113</v>
+        <v>9.10499382019043</v>
       </c>
       <c r="AO10" t="n">
         <v>10.51279544830322</v>
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>31.3927173614502</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>3.578455209732056</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>3.693013191223145</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.812335014343262</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>4.032497882843018</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>4.28525972366333</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.871307373046875</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.9318528175354</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.373353004455566</v>
       </c>
     </row>
     <row r="11">
@@ -1746,88 +1966,88 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.441414194762573</v>
+        <v>4.441412691700473</v>
       </c>
       <c r="D11" t="n">
-        <v>2.675506087585493</v>
+        <v>2.675506711366491</v>
       </c>
       <c r="E11" t="n">
-        <v>4.572576157270068</v>
+        <v>4.572576958886569</v>
       </c>
       <c r="F11" t="n">
-        <v>4.946029266035273</v>
+        <v>4.946029945668114</v>
       </c>
       <c r="G11" t="n">
-        <v>5.513410848107911</v>
+        <v>5.513411729639838</v>
       </c>
       <c r="H11" t="n">
-        <v>6.222868626521864</v>
+        <v>6.222869729542461</v>
       </c>
       <c r="I11" t="n">
-        <v>7.031393562748965</v>
+        <v>7.031394369947872</v>
       </c>
       <c r="J11" t="n">
-        <v>9.310902315410189</v>
+        <v>9.3109029552141</v>
       </c>
       <c r="K11" t="n">
-        <v>11.78703123637479</v>
+        <v>11.78703193927159</v>
       </c>
       <c r="L11" t="n">
-        <v>22.14579335447886</v>
+        <v>22.14579395296179</v>
       </c>
       <c r="M11" t="n">
-        <v>4.493873644333242</v>
+        <v>4.493873941155948</v>
       </c>
       <c r="N11" t="n">
-        <v>4.565425425839147</v>
+        <v>4.565425614782711</v>
       </c>
       <c r="O11" t="n">
-        <v>4.656004995762628</v>
+        <v>4.65600500137579</v>
       </c>
       <c r="P11" t="n">
-        <v>4.768035691987908</v>
+        <v>4.768036090609735</v>
       </c>
       <c r="Q11" t="n">
-        <v>4.898999594109851</v>
+        <v>4.898998920145972</v>
       </c>
       <c r="R11" t="n">
-        <v>5.312017831117284</v>
+        <v>5.312018698868376</v>
       </c>
       <c r="S11" t="n">
-        <v>5.859301599137753</v>
+        <v>5.85930188782088</v>
       </c>
       <c r="T11" t="n">
-        <v>8.975118510649704</v>
+        <v>8.975118931338361</v>
       </c>
       <c r="U11" t="n">
-        <v>4.572576157270068</v>
+        <v>4.572576958886569</v>
       </c>
       <c r="V11" t="n">
-        <v>4.953200820994147</v>
+        <v>4.953201241348698</v>
       </c>
       <c r="W11" t="n">
-        <v>5.529108362529353</v>
+        <v>5.529108505688868</v>
       </c>
       <c r="X11" t="n">
-        <v>6.249426106848284</v>
+        <v>6.249427282216861</v>
       </c>
       <c r="Y11" t="n">
-        <v>7.068373382799417</v>
+        <v>7.068373322535932</v>
       </c>
       <c r="Z11" t="n">
-        <v>8.901565128095317</v>
+        <v>8.90156547968955</v>
       </c>
       <c r="AA11" t="n">
-        <v>11.89270659256736</v>
+        <v>11.89270631805088</v>
       </c>
       <c r="AB11" t="n">
-        <v>22.30924083079574</v>
+        <v>22.30924114478159</v>
       </c>
       <c r="AC11" t="n">
-        <v>5.477431550775657</v>
+        <v>5.477431724885419</v>
       </c>
       <c r="AD11" t="n">
-        <v>6.637193794155904</v>
+        <v>6.637193506783148</v>
       </c>
       <c r="AE11" t="n">
         <v>7.866320716664916</v>
@@ -1839,28 +2059,28 @@
         <v>10.43113139583936</v>
       </c>
       <c r="AH11" t="n">
-        <v>13.72631071464437</v>
+        <v>13.72631127046702</v>
       </c>
       <c r="AI11" t="n">
         <v>17.05511784414679</v>
       </c>
       <c r="AJ11" t="n">
-        <v>30.21620901286882</v>
+        <v>30.21621002284256</v>
       </c>
       <c r="AK11" t="n">
-        <v>5.601556030439953</v>
+        <v>5.601555860188272</v>
       </c>
       <c r="AL11" t="n">
         <v>6.857056940766645</v>
       </c>
       <c r="AM11" t="n">
-        <v>8.164794188204757</v>
+        <v>8.164793720991833</v>
       </c>
       <c r="AN11" t="n">
         <v>9.503233509893077</v>
       </c>
       <c r="AO11" t="n">
-        <v>10.85996970325269</v>
+        <v>10.85997075703936</v>
       </c>
       <c r="AP11" t="n">
         <v>14.29750841749157</v>
@@ -1869,7 +2089,31 @@
         <v>17.7638590261238</v>
       </c>
       <c r="AR11" t="n">
-        <v>31.60565486481167</v>
+        <v>31.60565196809148</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>4.537295603286341</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4.66846170416204</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>4.783564387643635</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>5.065537471591601</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>5.352594741061211</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6.231682140857916</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>7.453490434240881</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>11.64278044746407</v>
       </c>
     </row>
     <row r="12">
@@ -1880,7 +2124,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9997792840003967</v>
+        <v>0.9997790455818176</v>
       </c>
       <c r="D12" t="n">
         <v>0.999869167804718</v>
@@ -1892,19 +2136,19 @@
         <v>0.9997055530548096</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9996033906936646</v>
+        <v>0.999603271484375</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9994574189186096</v>
+        <v>0.9994571805000305</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9992675185203552</v>
+        <v>0.9992673993110657</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9986018538475037</v>
+        <v>0.9986015558242798</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9976651668548584</v>
+        <v>0.9976649284362793</v>
       </c>
       <c r="L12" t="n">
         <v>0.9913324117660522</v>
@@ -1913,49 +2157,49 @@
         <v>0.9997753500938416</v>
       </c>
       <c r="N12" t="n">
-        <v>0.999768853187561</v>
+        <v>0.9997687339782715</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9997588992118835</v>
+        <v>0.9997589588165283</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9997456073760986</v>
+        <v>0.9997456669807434</v>
       </c>
       <c r="Q12" t="n">
         <v>0.9997292160987854</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9996724724769592</v>
+        <v>0.9996723532676697</v>
       </c>
       <c r="S12" t="n">
         <v>0.9995887279510498</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9989690780639648</v>
+        <v>0.9989689588546753</v>
       </c>
       <c r="U12" t="n">
         <v>0.999764084815979</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9997062683105469</v>
+        <v>0.9997060298919678</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9996066689491272</v>
+        <v>0.9996065497398376</v>
       </c>
       <c r="X12" t="n">
-        <v>0.999464213848114</v>
+        <v>0.9994640946388245</v>
       </c>
       <c r="Y12" t="n">
         <v>0.9992795586585999</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9987785816192627</v>
+        <v>0.9987784624099731</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.9977099895477295</v>
+        <v>0.9977098703384399</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.9915730357170105</v>
+        <v>0.9915729761123657</v>
       </c>
       <c r="AC12" t="n">
         <v>0.9996243119239807</v>
@@ -1964,37 +2208,37 @@
         <v>0.999402642250061</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.999113142490387</v>
+        <v>0.9991132616996765</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.9987556338310242</v>
+        <v>0.9987557530403137</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.9983307719230652</v>
+        <v>0.9983306527137756</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.9969691634178162</v>
+        <v>0.9969690442085266</v>
       </c>
       <c r="AI12" t="n">
         <v>0.9951816201210022</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.9840055704116821</v>
+        <v>0.9840054512023926</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.9996556043624878</v>
+        <v>0.9996554851531982</v>
       </c>
       <c r="AL12" t="n">
         <v>0.9994791150093079</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.9992486834526062</v>
+        <v>0.9992485642433167</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.9989631175994873</v>
+        <v>0.9989629983901978</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.9986222386360168</v>
+        <v>0.9986221194267273</v>
       </c>
       <c r="AP12" t="n">
         <v>0.9975172281265259</v>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9861145615577698</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997672438621521</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997512698173523</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997455477714539</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.999670147895813</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996466636657715</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9994515180587769</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9991946816444397</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9977099299430847</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>